<commit_message>
added user manager y recuperacion de usuarrio
</commit_message>
<xml_diff>
--- a/bin/Debug/inventario.xlsx
+++ b/bin/Debug/inventario.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Nalgas de tom</t>
   </si>
   <si>
+    <t>nalga de tom</t>
+  </si>
+  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -93,6 +96,27 @@
   </si>
   <si>
     <t>2025-08-04 14:55:21</t>
+  </si>
+  <si>
+    <t>2025-08-04 15:31:33</t>
+  </si>
+  <si>
+    <t>2025-08-04 15:32:06</t>
+  </si>
+  <si>
+    <t>2025-08-04 18:24:44</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Inicio de sesión</t>
+  </si>
+  <si>
+    <t>2025-08-04 18:40:02</t>
+  </si>
+  <si>
+    <t>2025-08-04 18:46:00</t>
   </si>
 </sst>
 </file>
@@ -411,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
@@ -460,7 +484,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="0">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D3" s="0">
         <v>4500</v>
@@ -534,6 +558,20 @@
       </c>
       <c r="D8" s="0">
         <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="0">
+        <v>99984</v>
+      </c>
+      <c r="D9" s="0">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +582,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5829B-F77D-405B-A283-69D8323B363B}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,33 +599,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
@@ -602,15 +640,15 @@
         <v>54000</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>7</v>
@@ -625,15 +663,15 @@
         <v>62400</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>7</v>
@@ -648,15 +686,15 @@
         <v>62400</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>9</v>
@@ -671,15 +709,15 @@
         <v>105000</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>10</v>
@@ -694,7 +732,122 @@
         <v>200</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0">
+        <v>-10</v>
+      </c>
+      <c r="E7" s="0">
+        <v>4500</v>
+      </c>
+      <c r="F7" s="0">
+        <v>45000</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="0">
+        <v>-16</v>
+      </c>
+      <c r="E8" s="0">
+        <v>115</v>
+      </c>
+      <c r="F8" s="0">
+        <v>1840</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CSV export, backups, and encrypted user storage (#2)
</commit_message>
<xml_diff>
--- a/bin/Debug/inventario.xlsx
+++ b/bin/Debug/inventario.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -147,6 +147,33 @@
   </si>
   <si>
     <t>2025-08-04 19:57:22</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:28:40</t>
+  </si>
+  <si>
+    <t>Blestro</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:31:26</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:31:31</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:31:40</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:31:45</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:31:58</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:32:19</t>
+  </si>
+  <si>
+    <t>2025-08-04 20:32:29</t>
   </si>
 </sst>
 </file>
@@ -514,7 +541,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="0">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="D3" s="0">
         <v>4500</v>
@@ -542,7 +569,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0">
         <v>5200</v>
@@ -556,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="0">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="D6" s="0">
         <v>1000</v>
@@ -584,7 +611,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="0">
         <v>100</v>
@@ -598,7 +625,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="0">
-        <v>99884</v>
+        <v>99862</v>
       </c>
       <c r="D9" s="0">
         <v>115</v>
@@ -612,7 +639,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5829B-F77D-405B-A283-69D8323B363B}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1087,6 +1114,190 @@
         <v>29</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0">
+        <v>0</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="0">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="0">
+        <v>1000</v>
+      </c>
+      <c r="F22" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="0">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="0">
+        <v>4500</v>
+      </c>
+      <c r="F23" s="0">
+        <v>4500</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="0">
+        <v>-22</v>
+      </c>
+      <c r="E24" s="0">
+        <v>115</v>
+      </c>
+      <c r="F24" s="0">
+        <v>2530</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="0">
+        <v>-22</v>
+      </c>
+      <c r="E25" s="0">
+        <v>1000</v>
+      </c>
+      <c r="F25" s="0">
+        <v>22000</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="0">
+        <v>-2</v>
+      </c>
+      <c r="E26" s="0">
+        <v>100</v>
+      </c>
+      <c r="F26" s="0">
+        <v>200</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="0">
+        <v>-47</v>
+      </c>
+      <c r="E27" s="0">
+        <v>5200</v>
+      </c>
+      <c r="F27" s="0">
+        <v>244400</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="0">
+        <v>-47</v>
+      </c>
+      <c r="E28" s="0">
+        <v>4500</v>
+      </c>
+      <c r="F28" s="0">
+        <v>211500</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>